<commit_message>
fix to have 23/24 data
</commit_message>
<xml_diff>
--- a/Data/dispensing_data_England_SW.xlsx
+++ b/Data/dispensing_data_England_SW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://southglos.sharepoint.com/sites/PublicHealthEvidencePerformanceandIntelligence/Shared Documents/JSNA/PNA 2025/pna_localities/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{D8DDF75E-57E6-4152-9960-FD8E3609AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95B9719A-A926-4573-B012-0BC5BF14C97E}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{D8DDF75E-57E6-4152-9960-FD8E3609AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AFD094D-C0C4-4AB4-94E0-223392E9E19C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB2C768B-C8FD-4358-97A6-DE8A0C4C14C5}"/>
+    <workbookView xWindow="-32914" yWindow="-7431" windowWidth="11237" windowHeight="17914" xr2:uid="{FB2C768B-C8FD-4358-97A6-DE8A0C4C14C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>England</t>
   </si>
   <si>
-    <t>2022/23</t>
-  </si>
-  <si>
     <t>fy</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>pop</t>
+  </si>
+  <si>
+    <t>2023/24</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,53 +456,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>5764881</v>
+        <v>5811259</v>
       </c>
       <c r="D2" s="1">
-        <v>1019</v>
+        <v>1107</v>
       </c>
       <c r="E2" s="1">
-        <v>97320582</v>
+        <v>99164702</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>57106398</v>
+        <v>57690323</v>
       </c>
       <c r="D3" s="1">
-        <v>11414</v>
+        <v>12009</v>
       </c>
       <c r="E3" s="2">
-        <v>1078984056</v>
+        <v>1112920890</v>
       </c>
     </row>
   </sheetData>
@@ -512,6 +512,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Sensitivedata xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">false</Sensitivedata>
+    <Retention_x0020_end_x0020_date xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b4ff75f0-9bd5-40ee-9010-33523d454cfa" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Notes xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F245FD19D15EEB4F856804E30AE6C910" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c46255a99c72d0de6965ece9445551b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xmlns:ns3="53d9a618-c0fc-4378-be70-69d4cc9b9182" xmlns:ns4="b4ff75f0-9bd5-40ee-9010-33523d454cfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98ddafb2fddb26920fa32bfe788e6dc1" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
@@ -779,37 +802,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Sensitivedata xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">false</Sensitivedata>
-    <Retention_x0020_end_x0020_date xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b4ff75f0-9bd5-40ee-9010-33523d454cfa" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Notes xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5665F80-64F8-4491-9FF8-93C70EB1D5FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44C46CD3-F384-4B27-9466-6B774B00D3F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
+    <ds:schemaRef ds:uri="b4ff75f0-9bd5-40ee-9010-33523d454cfa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A473D1B-9122-422C-8CE6-64A46C1F5629}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A473D1B-9122-422C-8CE6-64A46C1F5629}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44C46CD3-F384-4B27-9466-6B774B00D3F0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5665F80-64F8-4491-9FF8-93C70EB1D5FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
+    <ds:schemaRef ds:uri="53d9a618-c0fc-4378-be70-69d4cc9b9182"/>
+    <ds:schemaRef ds:uri="b4ff75f0-9bd5-40ee-9010-33523d454cfa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add LA to provision table
</commit_message>
<xml_diff>
--- a/Data/dispensing_data_England_SW.xlsx
+++ b/Data/dispensing_data_England_SW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://southglos.sharepoint.com/sites/PublicHealthEvidencePerformanceandIntelligence/Shared Documents/JSNA/PNA 2025/pna_localities/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{D8DDF75E-57E6-4152-9960-FD8E3609AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AFD094D-C0C4-4AB4-94E0-223392E9E19C}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{D8DDF75E-57E6-4152-9960-FD8E3609AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{655471E4-B092-4A3F-8EE9-AE015AD9C326}"/>
   <bookViews>
-    <workbookView xWindow="-32914" yWindow="-7431" windowWidth="11237" windowHeight="17914" xr2:uid="{FB2C768B-C8FD-4358-97A6-DE8A0C4C14C5}"/>
+    <workbookView xWindow="-27531" yWindow="-5623" windowWidth="22208" windowHeight="12266" xr2:uid="{FB2C768B-C8FD-4358-97A6-DE8A0C4C14C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>South West</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>n_items</t>
-  </si>
-  <si>
-    <t>pop</t>
   </si>
   <si>
     <t>2023/24</t>
@@ -440,21 +437,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE5E660-6A70-499A-ADBD-FCDF7F4B0D0E}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -462,46 +458,37 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>5811259</v>
+        <v>1107</v>
       </c>
       <c r="D2" s="1">
-        <v>1107</v>
-      </c>
-      <c r="E2" s="1">
         <v>99164702</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>57690323</v>
-      </c>
-      <c r="D3" s="1">
         <v>12009</v>
       </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2">
         <v>1112920890</v>
       </c>
     </row>
@@ -512,29 +499,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Sensitivedata xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">false</Sensitivedata>
-    <Retention_x0020_end_x0020_date xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b4ff75f0-9bd5-40ee-9010-33523d454cfa" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Notes xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F245FD19D15EEB4F856804E30AE6C910" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c46255a99c72d0de6965ece9445551b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xmlns:ns3="53d9a618-c0fc-4378-be70-69d4cc9b9182" xmlns:ns4="b4ff75f0-9bd5-40ee-9010-33523d454cfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98ddafb2fddb26920fa32bfe788e6dc1" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
@@ -802,26 +766,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Sensitivedata xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">false</Sensitivedata>
+    <Retention_x0020_end_x0020_date xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b4ff75f0-9bd5-40ee-9010-33523d454cfa" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Notes xmlns="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44C46CD3-F384-4B27-9466-6B774B00D3F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
-    <ds:schemaRef ds:uri="b4ff75f0-9bd5-40ee-9010-33523d454cfa"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A473D1B-9122-422C-8CE6-64A46C1F5629}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5665F80-64F8-4491-9FF8-93C70EB1D5FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -839,4 +807,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A473D1B-9122-422C-8CE6-64A46C1F5629}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44C46CD3-F384-4B27-9466-6B774B00D3F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2cb04cb6-fd46-45ab-a0b1-cdeedec8e6ae"/>
+    <ds:schemaRef ds:uri="b4ff75f0-9bd5-40ee-9010-33523d454cfa"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>